<commit_message>
prepare release & message f7cca33308aaf42375b861b8535c0d9cf2bad208
</commit_message>
<xml_diff>
--- a/nr-update-menu/ig/CodeSystem-competence-code-system.xlsx
+++ b/nr-update-menu/ig/CodeSystem-competence-code-system.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>0.1.0-ballot</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-11-14T14:16:48+00:00</t>
+    <t>2024-11-15T13:53:55+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>